<commit_message>
upates to my picks locked and leaderboard pages are complete
</commit_message>
<xml_diff>
--- a/excel docs/lifecycle info.xlsx
+++ b/excel docs/lifecycle info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C87284A-4256-B14D-81D4-E31A1C65F307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265C5988-5DF6-BE43-80A2-1806A198306A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="15880" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="96">
   <si>
     <t>need to submit a number for tiebreaker score</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Pre Tourney - before part makes their picks</t>
   </si>
   <si>
-    <t>Admin_Page: only viewable to joe</t>
-  </si>
-  <si>
     <t>Header_P: audit header for all tabs</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t>My_Picks_Page_Unlocked: all pages are not accesable</t>
   </si>
   <si>
-    <t>Leaderboard_Page: hide the Scorecard_Cont</t>
-  </si>
-  <si>
     <t>Leaderboard_Page: un-hide the Leaderboard_Cont</t>
   </si>
   <si>
@@ -324,6 +318,12 @@
   </si>
   <si>
     <t>Pool_Picks_Page: un-hide the "box left" tag which allows you to view other parts picks</t>
+  </si>
+  <si>
+    <t>Leaderboard_Page: hide the Leaderboard_Cont</t>
+  </si>
+  <si>
+    <t>Admin_Pages: only viewable to joe</t>
   </si>
 </sst>
 </file>
@@ -892,11 +892,9 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -912,7 +910,7 @@
       </c>
       <c r="E1" s="10"/>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -926,7 +924,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="B3" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -968,85 +966,85 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="30"/>
       <c r="B10" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="30"/>
       <c r="B11" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="30"/>
       <c r="B12" s="23" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="30"/>
-      <c r="B13" s="26" t="s">
-        <v>57</v>
+      <c r="B13" s="23" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="30"/>
       <c r="B14" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="30"/>
       <c r="B15" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="30"/>
       <c r="B16" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="30"/>
       <c r="B17" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="30"/>
       <c r="B18" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="30"/>
       <c r="B19" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="30"/>
       <c r="B20" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="30"/>
       <c r="B21" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="30"/>
       <c r="B22" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="30"/>
       <c r="B23" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1058,97 +1056,97 @@
         <v>4</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="30"/>
       <c r="B26" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="30"/>
       <c r="B27" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="30"/>
       <c r="B28" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="30"/>
       <c r="B29" s="23" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="30"/>
-      <c r="B30" s="26" t="s">
-        <v>57</v>
+      <c r="B30" s="23" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="30"/>
       <c r="B31" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="30"/>
       <c r="B32" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="30"/>
       <c r="B33" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="30"/>
       <c r="B35" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="30"/>
       <c r="B36" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="30"/>
       <c r="B37" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="30"/>
       <c r="B38" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="30"/>
       <c r="B39" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="30"/>
       <c r="B40" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1158,27 +1156,27 @@
     <row r="42" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1188,73 +1186,73 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B49" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B50" s="23" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B51" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="23" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B53" s="26" t="s">
-        <v>58</v>
+      <c r="B53" s="23" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B54" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B55" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B56" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B57" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B58" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B59" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C59" s="12"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B60" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B61" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -1263,151 +1261,196 @@
     </row>
     <row r="63" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="B63" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B64" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="8"/>
+      <c r="B81" s="9"/>
+    </row>
+    <row r="82" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+      <c r="B82" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B84" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B68" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B69" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B70" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B71" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B72" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B73" s="25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B74" s="23" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B77" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="9"/>
-    </row>
-    <row r="79" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
-      <c r="B79" s="17" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="11" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B83" s="23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B84" s="26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B85" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B86" s="26" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="8"/>
+      <c r="B98" s="9"/>
+    </row>
+    <row r="99" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A99" s="13"/>
+      <c r="B99" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B87" s="26" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B88" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="8"/>
-      <c r="B89" s="9"/>
-    </row>
-    <row r="90" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
-      <c r="B90" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B91" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B92" s="18" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B101" s="18" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1456,7 +1499,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>20</v>
@@ -1474,7 +1517,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>20</v>
@@ -1499,7 +1542,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>20</v>
@@ -1516,7 +1559,7 @@
       <c r="A9" s="36"/>
       <c r="B9" s="37"/>
       <c r="C9" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1524,7 +1567,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>20</v>
@@ -1540,7 +1583,7 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
       <c r="B12" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="31"/>
     </row>
@@ -1600,7 +1643,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1610,17 +1653,17 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1635,7 +1678,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1643,17 +1686,17 @@
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="19" x14ac:dyDescent="0.25">
@@ -1668,12 +1711,12 @@
     </row>
     <row r="23" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hiding/showing containers based on tourneyStage work started, not complete yet
</commit_message>
<xml_diff>
--- a/excel docs/lifecycle info.xlsx
+++ b/excel docs/lifecycle info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE69FA0-5FCF-3847-A773-D5851B60E81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B974442-B002-D148-A36F-AF86A8CBF908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
   <si>
     <t>need to submit a number for tiebreaker score</t>
   </si>
@@ -140,9 +140,6 @@
     <t>copy all part data into this doc</t>
   </si>
   <si>
-    <t>change tourneyStage on Joe model to commenced</t>
-  </si>
-  <si>
     <t>once all finished, verify that you can change literally every value for this part</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>Pool_Picks_Page: hide everything</t>
   </si>
   <si>
-    <t>My_Picks_Unlocked: hide the knockout stuff</t>
-  </si>
-  <si>
     <t>My_Picks_Locked: show the parts picks - still have a button to edit</t>
   </si>
   <si>
@@ -197,18 +191,12 @@
     <t>Leaderboard_Page: un-hide the Leaderboard_Cont</t>
   </si>
   <si>
-    <t>change tourneyStage on Joe model to pre-ko</t>
-  </si>
-  <si>
     <t>update each team instance to reflect their group finishing position</t>
   </si>
   <si>
     <t>once KO stage commences</t>
   </si>
   <si>
-    <t>change tourneyStage on Joe model to ko</t>
-  </si>
-  <si>
     <t>After each game in KO</t>
   </si>
   <si>
@@ -260,30 +248,15 @@
     <t>My_Picks_Locked: The edit button says Group, not Knockout</t>
   </si>
   <si>
-    <t>My_Picks_Locked: part can only view the group picks, aka no KO info</t>
-  </si>
-  <si>
-    <t>My_Picks_Locked: group points color coded table is showing now in the header cont</t>
-  </si>
-  <si>
-    <t>My_Picks_Locked: group points color coded table is showing in the header cont</t>
-  </si>
-  <si>
     <t>My_Picks_Page_Locked: edit picks button is disabled</t>
   </si>
   <si>
-    <t>My_Picks_Page_Unlocked: only shows the KO info to edit</t>
-  </si>
-  <si>
     <t>My_Picks_Locked: un-hide the KO bracket info</t>
   </si>
   <si>
     <t>My_Picks_Locked: edit button says Knockout, not Group</t>
   </si>
   <si>
-    <t>My_Picks_Locked: group points color coded table is not in the header anymore, and is in between the KO bracket and group pick info</t>
-  </si>
-  <si>
     <t>My_Picks_Locked: total point info on the right is hidden</t>
   </si>
   <si>
@@ -312,6 +285,24 @@
   </si>
   <si>
     <t>Pool_Picks_Page: right side hide total point info in the group row</t>
+  </si>
+  <si>
+    <t>change tourneyStage on Joe model to "commenced"</t>
+  </si>
+  <si>
+    <t>change tourneyStage on Joe model to "pre-ko"</t>
+  </si>
+  <si>
+    <t>change tourneyStage on Joe model to "ko"</t>
+  </si>
+  <si>
+    <t>My_Picks_Unlocked: ko edit page is not accesable</t>
+  </si>
+  <si>
+    <t>My_Picks_Page_Unlocked: only shows the KO info to edit - group edit page not accesible</t>
+  </si>
+  <si>
+    <t>My_Picks_Locked: group points color coded table is in between the KO bracket and group pick info</t>
   </si>
 </sst>
 </file>
@@ -368,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,12 +393,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -527,7 +512,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -555,7 +540,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,9 +862,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -910,7 +896,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="26"/>
       <c r="B3" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -964,55 +950,55 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="22" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="22" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="22" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="22" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
-      <c r="B19" s="25" t="s">
-        <v>72</v>
+      <c r="B19" s="22" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1030,7 +1016,7 @@
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1048,25 +1034,25 @@
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="22" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="22" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1078,314 +1064,297 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="22" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="22" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="27"/>
-      <c r="B33" s="25" t="s">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+    </row>
+    <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="27"/>
-      <c r="B34" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9"/>
-    </row>
-    <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16" t="s">
-        <v>48</v>
+      <c r="B35" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="17" t="s">
-        <v>33</v>
+      <c r="B37" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="11" t="s">
-        <v>50</v>
+      <c r="B40" s="22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="11" t="s">
-        <v>21</v>
+      <c r="B41" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" s="22" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="22" t="s">
-        <v>28</v>
+      <c r="B43" s="23" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="22" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="23" t="s">
-        <v>32</v>
+      <c r="B45" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="22" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="22" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="22" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B49" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B50" s="22" t="s">
-        <v>77</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C50" s="12"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B51" s="22" t="s">
-        <v>83</v>
+      <c r="B51" s="25" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B52" s="22" t="s">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B53" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B54" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B53" s="25" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B55" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="12"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B54" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="8"/>
-      <c r="B55" s="9"/>
-    </row>
-    <row r="56" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="B56" s="16" t="s">
-        <v>68</v>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B56" s="17" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B57" s="11" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B58" s="17" t="s">
-        <v>54</v>
+      <c r="B58" s="22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B59" s="17" t="s">
-        <v>21</v>
+      <c r="B59" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B60" s="11" t="s">
-        <v>69</v>
+      <c r="B60" s="22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B61" s="22" t="s">
-        <v>27</v>
+      <c r="B61" s="23" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B62" s="22" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B63" s="22" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B64" s="23" t="s">
-        <v>32</v>
+      <c r="B64" s="24" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="22" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B67" s="24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B68" s="24" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B69" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B70" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B71" s="25" t="s">
-        <v>78</v>
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+    </row>
+    <row r="71" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B72" s="24" t="s">
-        <v>88</v>
+      <c r="B72" s="11" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="8"/>
-      <c r="B73" s="9"/>
-    </row>
-    <row r="74" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
-      <c r="B74" s="16" t="s">
-        <v>55</v>
+      <c r="B73" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="11" t="s">
-        <v>56</v>
+      <c r="B75" s="22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B76" s="22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" s="22" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B78" s="22" t="s">
-        <v>27</v>
+      <c r="B78" s="23" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" s="22" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B80" s="22" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="23" t="s">
-        <v>32</v>
+      <c r="B81" s="22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" s="22" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B83" s="22" t="s">
-        <v>52</v>
+      <c r="B83" s="24" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B84" s="22" t="s">
-        <v>71</v>
+      <c r="B84" s="24" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B85" s="25" t="s">
-        <v>51</v>
+      <c r="B85" s="24" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B86" s="24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B87" s="24" t="s">
-        <v>91</v>
+      <c r="A86" s="8"/>
+      <c r="B86" s="9"/>
+    </row>
+    <row r="87" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" s="13"/>
+      <c r="B87" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B88" s="24" t="s">
-        <v>90</v>
+      <c r="B88" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="8"/>
-      <c r="B89" s="9"/>
-    </row>
-    <row r="90" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
-      <c r="B90" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B91" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B92" s="17" t="s">
+      <c r="B89" s="17" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1393,7 +1362,7 @@
   <mergeCells count="3">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A9:A20"/>
-    <mergeCell ref="A22:A34"/>
+    <mergeCell ref="A22:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1434,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>20</v>
@@ -1452,7 +1421,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>20</v>
@@ -1477,7 +1446,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>20</v>
@@ -1494,7 +1463,7 @@
       <c r="A9" s="33"/>
       <c r="B9" s="34"/>
       <c r="C9" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1502,7 +1471,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>20</v>
@@ -1518,7 +1487,7 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="33"/>
       <c r="B12" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="28"/>
     </row>
@@ -1578,7 +1547,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1588,17 +1557,17 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1613,7 +1582,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1621,17 +1590,17 @@
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="19" x14ac:dyDescent="0.25">
@@ -1646,12 +1615,12 @@
     </row>
     <row r="23" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
my picks unlocked page work is complete
</commit_message>
<xml_diff>
--- a/excel docs/lifecycle info.xlsx
+++ b/excel docs/lifecycle info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3906DC51-C67A-9F4A-B075-62B2F3ED099B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE172CD-3B8E-0640-B7FD-EDFA59694C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="2" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
@@ -885,7 +885,7 @@
   </sheetPr>
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0"/>
+    <sheetView topLeftCell="A55" zoomScale="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1622,8 +1622,8 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
payout info added, create account feature hidden if stage !== 1, server notes updated
</commit_message>
<xml_diff>
--- a/excel docs/lifecycle info.xlsx
+++ b/excel docs/lifecycle info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F318A26C-B46E-1E4D-863C-6B32B1AF6C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E0BEE5-4F9B-B445-ACD3-7514E37F35BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-6540" windowWidth="21600" windowHeight="37900" activeTab="2" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18600" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="91">
   <si>
     <t>need to submit a number for tiebreaker score</t>
   </si>
@@ -159,12 +159,6 @@
   </si>
   <si>
     <t>Once WC commences</t>
-  </si>
-  <si>
-    <t>create a const for each team to findOne</t>
-  </si>
-  <si>
-    <t>create a promise all to save each team</t>
   </si>
   <si>
     <t>My_Picks_Page_Unlocked: all pages are not accesable</t>
@@ -522,31 +516,31 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -874,9 +868,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -896,7 +892,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="25">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -904,19 +900,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="25"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="18" t="s">
         <v>18</v>
       </c>
@@ -938,7 +934,7 @@
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="26">
+      <c r="A9" s="27">
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -946,67 +942,67 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="21" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="27"/>
+      <c r="B17" s="21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="26"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="26"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="21" t="s">
         <v>38</v>
       </c>
@@ -1016,7 +1012,7 @@
       <c r="B21" s="9"/>
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="26">
+      <c r="A22" s="27">
         <v>4</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -1024,436 +1020,421 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="26"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="26"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="26"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="26"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="26"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="26"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="21" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="26"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="26"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="26"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="26"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
     </row>
-    <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B35" s="17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B41" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B47" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="12"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B48" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+      <c r="B49" s="9"/>
+    </row>
+    <row r="50" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B50" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B59" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B60" s="23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B61" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B62" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B63" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
+      <c r="B64" s="9"/>
+    </row>
+    <row r="65" spans="2:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B65" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="11" t="s">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="21" t="s">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="12"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B51" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="9"/>
-    </row>
-    <row r="53" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="B53" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B54" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B55" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B56" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B57" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B58" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B59" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B60" s="22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B61" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B62" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B63" s="23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B64" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="8"/>
-      <c r="B67" s="9"/>
-    </row>
-    <row r="68" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B68" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B69" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B70" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B71" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B72" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B73" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B74" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B77" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B78" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B79" s="23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="23" t="s">
-        <v>86</v>
-      </c>
-    </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="23" t="s">
-        <v>87</v>
+      <c r="B81" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" s="23" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B83" s="23" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B84" s="21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B85" s="23" t="s">
-        <v>89</v>
+      <c r="A84" s="8"/>
+      <c r="B84" s="9"/>
+    </row>
+    <row r="85" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A85" s="13"/>
+      <c r="B85" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B86" s="23" t="s">
-        <v>73</v>
+      <c r="B86" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="8"/>
-      <c r="B87" s="9"/>
-    </row>
-    <row r="88" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A88" s="13"/>
-      <c r="B88" s="16" t="s">
-        <v>46</v>
+      <c r="B87" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="21" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B89" s="11" t="s">
-        <v>82</v>
+      <c r="B89" s="21" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B90" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B91" s="21" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B92" s="21" t="s">
-        <v>24</v>
+      <c r="B92" s="22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" s="21" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B94" s="21" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B95" s="22" t="s">
-        <v>29</v>
+      <c r="B95" s="21" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B96" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B97" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="21" t="s">
-        <v>61</v>
+      <c r="B98" s="23" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="21" t="s">
-        <v>43</v>
+      <c r="B99" s="23" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B100" s="23" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="23" t="s">
-        <v>88</v>
+      <c r="A101" s="8"/>
+      <c r="B101" s="9"/>
+    </row>
+    <row r="102" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A102" s="13"/>
+      <c r="B102" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B103" s="23" t="s">
-        <v>89</v>
+      <c r="B103" s="17" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="8"/>
-      <c r="B104" s="9"/>
-    </row>
-    <row r="105" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A105" s="13"/>
-      <c r="B105" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B106" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B107" s="17" t="s">
+      <c r="B104" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1498,65 +1479,65 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="25" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="25" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="25" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>91</v>
+      <c r="C6" s="25" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="34"/>
-      <c r="B8" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="33"/>
+      <c r="B8" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1579,7 +1560,7 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1612,7 +1593,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1627,12 +1608,12 @@
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1647,7 +1628,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1655,17 +1636,17 @@
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="19" x14ac:dyDescent="0.25">
@@ -1680,12 +1661,12 @@
     </row>
     <row r="23" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started on re-doing UserAccount stuff
</commit_message>
<xml_diff>
--- a/excel docs/lifecycle info.xlsx
+++ b/excel docs/lifecycle info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joecollins/Desktop/documents/personal-projects/world-cup-heroku/excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084F02D5-2751-4542-8953-5E1CECD4F60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545F06FF-5BCD-8345-B608-25195B8CF610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47300" yWindow="-3080" windowWidth="23760" windowHeight="18600" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{D89656BD-B983-D041-A997-C1184058734E}"/>
   </bookViews>
   <sheets>
     <sheet name="life cycle actions" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
   <si>
     <t>need to submit a number for tiebreaker score</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>My_Picks_Locked: right side hide total point info is in the ko picks row</t>
+  </si>
+  <si>
+    <t>Routes folder: comment out the Create_Account_Page</t>
   </si>
 </sst>
 </file>
@@ -519,6 +522,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,10 +553,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,10 +875,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="160" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,7 +899,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -904,19 +907,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="18" t="s">
         <v>18</v>
       </c>
@@ -938,7 +941,7 @@
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="A9" s="28">
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -946,68 +949,68 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="32" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="32" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="32" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="23" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="32" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="23" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="32" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="32" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="23" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="32" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
-      <c r="B17" s="32" t="s">
+      <c r="A17" s="28"/>
+      <c r="B17" s="23" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="32" t="s">
+      <c r="A18" s="28"/>
+      <c r="B18" s="23" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="32" t="s">
+      <c r="A19" s="28"/>
+      <c r="B19" s="23" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="32" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1016,7 +1019,7 @@
       <c r="B21" s="9"/>
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="24">
+      <c r="A22" s="28">
         <v>4</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -1024,50 +1027,50 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="32" t="s">
+      <c r="A24" s="28"/>
+      <c r="B24" s="23" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
-      <c r="B25" s="32" t="s">
+      <c r="A25" s="28"/>
+      <c r="B25" s="23" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="32" t="s">
+      <c r="A26" s="28"/>
+      <c r="B26" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="32" t="s">
+      <c r="A27" s="28"/>
+      <c r="B27" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
-      <c r="B28" s="32" t="s">
+      <c r="A28" s="28"/>
+      <c r="B28" s="23" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="24"/>
-      <c r="B29" s="32" t="s">
+      <c r="A29" s="28"/>
+      <c r="B29" s="23" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="32" t="s">
+      <c r="A30" s="28"/>
+      <c r="B30" s="23" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1082,306 +1085,312 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="13"/>
       <c r="B33" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="17" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B34" s="11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B36" s="17" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B37" s="32" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B38" s="33" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B39" s="32" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B40" s="32" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B41" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B41" s="32" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B42" s="32" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B43" s="32" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="32" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B45" s="32" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="12"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B46" s="34" t="s">
+      <c r="C46" s="12"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B47" s="25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-      <c r="B47" s="9"/>
-    </row>
-    <row r="48" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="B48" s="16" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="9"/>
+    </row>
+    <row r="49" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B49" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="11" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="11" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B51" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="32" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="33" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B54" s="32" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="32" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="35" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="32" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B58" s="35" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B59" s="26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B59" s="35" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B60" s="26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="8"/>
-      <c r="B60" s="9"/>
-    </row>
-    <row r="61" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B61" s="16" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="8"/>
+      <c r="B61" s="9"/>
+    </row>
+    <row r="62" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B62" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B62" s="11" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B63" s="11" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B63" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="11" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="32" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B67" s="33" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B68" s="32" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B69" s="32" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B70" s="35" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B71" s="35" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B72" s="35" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B73" s="35" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="26" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B74" s="35" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="32" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="35" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="8"/>
-      <c r="B77" s="9"/>
-    </row>
-    <row r="78" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
-      <c r="B78" s="16" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="8"/>
+      <c r="B78" s="9"/>
+    </row>
+    <row r="79" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B79" s="11" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="32" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="33" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="21" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B83" s="32" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B84" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B84" s="32" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B85" s="32" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B86" s="35" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B87" s="35" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="26" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B88" s="35" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B89" s="35" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="8"/>
-      <c r="B90" s="9"/>
-    </row>
-    <row r="91" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A91" s="13"/>
-      <c r="B91" s="15" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="8"/>
+      <c r="B91" s="9"/>
+    </row>
+    <row r="92" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A92" s="13"/>
+      <c r="B92" s="15" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B92" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1426,10 +1435,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>89</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -1437,17 +1446,17 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="32" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -1455,17 +1464,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="22" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="32" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -1473,18 +1482,18 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>